<commit_message>
Updated SO2 mapping for Europe.
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/EMEP_NFR09_scaling_mapping_SO2.xlsx
+++ b/input/mappings/scaling/EMEP_NFR09_scaling_mapping_SO2.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="800" yWindow="0" windowWidth="24400" windowHeight="13680" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="131">
   <si>
     <t>pre_ext_method</t>
   </si>
@@ -326,7 +326,94 @@
     <t>constant</t>
   </si>
   <si>
-    <t>Road</t>
+    <t>fin</t>
+  </si>
+  <si>
+    <t>Don't scale 1981 to avoid reporting mistake in inventory</t>
+  </si>
+  <si>
+    <t>lux</t>
+  </si>
+  <si>
+    <t>Avoid imlied Nox EF dip 1986-1989</t>
+  </si>
+  <si>
+    <t>(Better match to inventory if don't use linear to 1 for hun, bgr, gbr ind/power)</t>
+  </si>
+  <si>
+    <t>aut</t>
+  </si>
+  <si>
+    <t>bel</t>
+  </si>
+  <si>
+    <t>che</t>
+  </si>
+  <si>
+    <t>cyp</t>
+  </si>
+  <si>
+    <t>cze</t>
+  </si>
+  <si>
+    <t>deu</t>
+  </si>
+  <si>
+    <t>dnk</t>
+  </si>
+  <si>
+    <t>esp</t>
+  </si>
+  <si>
+    <t>est</t>
+  </si>
+  <si>
+    <t>fra</t>
+  </si>
+  <si>
+    <t>gbr</t>
+  </si>
+  <si>
+    <t>geo</t>
+  </si>
+  <si>
+    <t>hrv</t>
+  </si>
+  <si>
+    <t>irl</t>
+  </si>
+  <si>
+    <t>isl</t>
+  </si>
+  <si>
+    <t>ita</t>
+  </si>
+  <si>
+    <t>ltu</t>
+  </si>
+  <si>
+    <t>lva</t>
+  </si>
+  <si>
+    <t>nld</t>
+  </si>
+  <si>
+    <t>nor</t>
+  </si>
+  <si>
+    <t>pol</t>
+  </si>
+  <si>
+    <t>prt</t>
+  </si>
+  <si>
+    <t>rou</t>
+  </si>
+  <si>
+    <t>svk</t>
+  </si>
+  <si>
+    <t>swe</t>
   </si>
 </sst>
 </file>
@@ -382,8 +469,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="239">
+  <cellStyleXfs count="243">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -630,7 +721,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="239">
+  <cellStyles count="243">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -750,6 +841,8 @@
     <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -869,6 +962,8 @@
     <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1205,8 +1300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F128"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2098,10 +2193,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G108"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD5"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89:XFD90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2111,7 +2206,7 @@
     <col min="5" max="5" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2119,96 +2214,2159 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
         <v>65</v>
       </c>
-      <c r="C2" t="s">
-        <v>98</v>
+      <c r="C2">
+        <v>1970</v>
       </c>
       <c r="D2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F2">
-        <v>1970</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>99</v>
+      </c>
+      <c r="F2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C3" t="s">
-        <v>98</v>
+        <v>84</v>
+      </c>
+      <c r="C3">
+        <v>1970</v>
       </c>
       <c r="D3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F3">
-        <v>1970</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>99</v>
+      </c>
+      <c r="F3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
         <v>56</v>
       </c>
-      <c r="C4" t="s">
-        <v>98</v>
+      <c r="C4">
+        <v>1970</v>
       </c>
       <c r="D4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F4">
-        <v>1970</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>99</v>
+      </c>
+      <c r="F4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="B5" t="s">
         <v>55</v>
       </c>
-      <c r="C5" t="s">
-        <v>98</v>
+      <c r="C5">
+        <v>1970</v>
       </c>
       <c r="D5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
-      </c>
-      <c r="F5">
-        <v>1970</v>
+        <v>99</v>
+      </c>
+      <c r="F5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6">
+        <v>1970</v>
+      </c>
+      <c r="D6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7">
+        <v>1970</v>
+      </c>
+      <c r="D7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8">
+        <v>1970</v>
+      </c>
+      <c r="D8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9">
+        <v>1970</v>
+      </c>
+      <c r="D9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10">
+        <v>1970</v>
+      </c>
+      <c r="D10" t="s">
+        <v>98</v>
+      </c>
+      <c r="E10" t="s">
+        <v>99</v>
+      </c>
+      <c r="F10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11">
+        <v>1970</v>
+      </c>
+      <c r="D11" t="s">
+        <v>98</v>
+      </c>
+      <c r="E11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12">
+        <v>1970</v>
+      </c>
+      <c r="D12" t="s">
+        <v>98</v>
+      </c>
+      <c r="E12" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13">
+        <v>1970</v>
+      </c>
+      <c r="D13" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13" t="s">
+        <v>99</v>
+      </c>
+      <c r="F13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14">
+        <v>1970</v>
+      </c>
+      <c r="D14" t="s">
+        <v>98</v>
+      </c>
+      <c r="E14" t="s">
+        <v>99</v>
+      </c>
+      <c r="F14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15">
+        <v>1970</v>
+      </c>
+      <c r="D15" t="s">
+        <v>98</v>
+      </c>
+      <c r="E15" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16">
+        <v>1970</v>
+      </c>
+      <c r="D16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" t="s">
+        <v>99</v>
+      </c>
+      <c r="F16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17">
+        <v>1970</v>
+      </c>
+      <c r="D17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" t="s">
+        <v>99</v>
+      </c>
+      <c r="F17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>110</v>
+      </c>
+      <c r="B18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18">
+        <v>1990</v>
+      </c>
+      <c r="D18" t="s">
+        <v>98</v>
+      </c>
+      <c r="E18" t="s">
+        <v>99</v>
+      </c>
+      <c r="F18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19">
+        <v>1990</v>
+      </c>
+      <c r="D19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20">
+        <v>1990</v>
+      </c>
+      <c r="D20" t="s">
+        <v>98</v>
+      </c>
+      <c r="E20" t="s">
+        <v>99</v>
+      </c>
+      <c r="F20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>110</v>
+      </c>
+      <c r="B21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21">
+        <v>1990</v>
+      </c>
+      <c r="D21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E21" t="s">
+        <v>99</v>
+      </c>
+      <c r="F21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>111</v>
+      </c>
+      <c r="B22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22">
+        <v>1970</v>
+      </c>
+      <c r="D22" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" t="s">
+        <v>99</v>
+      </c>
+      <c r="F22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23">
+        <v>1970</v>
+      </c>
+      <c r="D23" t="s">
+        <v>98</v>
+      </c>
+      <c r="E23" t="s">
+        <v>99</v>
+      </c>
+      <c r="F23" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24">
+        <v>1970</v>
+      </c>
+      <c r="D24" t="s">
+        <v>98</v>
+      </c>
+      <c r="E24" t="s">
+        <v>99</v>
+      </c>
+      <c r="F24" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25">
+        <v>1970</v>
+      </c>
+      <c r="D25" t="s">
+        <v>98</v>
+      </c>
+      <c r="E25" t="s">
+        <v>99</v>
+      </c>
+      <c r="F25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>112</v>
+      </c>
+      <c r="B26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26">
+        <v>1970</v>
+      </c>
+      <c r="D26" t="s">
+        <v>98</v>
+      </c>
+      <c r="E26" t="s">
+        <v>99</v>
+      </c>
+      <c r="F26" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>112</v>
+      </c>
+      <c r="B27" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27">
+        <v>1970</v>
+      </c>
+      <c r="D27" t="s">
+        <v>98</v>
+      </c>
+      <c r="E27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F27" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>112</v>
+      </c>
+      <c r="B28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28">
+        <v>1970</v>
+      </c>
+      <c r="D28" t="s">
+        <v>98</v>
+      </c>
+      <c r="E28" t="s">
+        <v>99</v>
+      </c>
+      <c r="F28" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29">
+        <v>1970</v>
+      </c>
+      <c r="D29" t="s">
+        <v>98</v>
+      </c>
+      <c r="E29" t="s">
+        <v>99</v>
+      </c>
+      <c r="F29" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>113</v>
+      </c>
+      <c r="B30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30">
+        <v>1970</v>
+      </c>
+      <c r="D30" t="s">
+        <v>98</v>
+      </c>
+      <c r="E30" t="s">
+        <v>99</v>
+      </c>
+      <c r="F30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31">
+        <v>1970</v>
+      </c>
+      <c r="D31" t="s">
+        <v>98</v>
+      </c>
+      <c r="E31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F31" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>113</v>
+      </c>
+      <c r="B32" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32">
+        <v>1970</v>
+      </c>
+      <c r="D32" t="s">
+        <v>98</v>
+      </c>
+      <c r="E32" t="s">
+        <v>99</v>
+      </c>
+      <c r="F32" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>113</v>
+      </c>
+      <c r="B33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33">
+        <v>1970</v>
+      </c>
+      <c r="D33" t="s">
+        <v>98</v>
+      </c>
+      <c r="E33" t="s">
+        <v>99</v>
+      </c>
+      <c r="F33" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>114</v>
+      </c>
+      <c r="B34" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34">
+        <v>1970</v>
+      </c>
+      <c r="D34" t="s">
+        <v>98</v>
+      </c>
+      <c r="E34" t="s">
+        <v>99</v>
+      </c>
+      <c r="F34" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35">
+        <v>1970</v>
+      </c>
+      <c r="D35" t="s">
+        <v>98</v>
+      </c>
+      <c r="E35" t="s">
+        <v>99</v>
+      </c>
+      <c r="F35" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>114</v>
+      </c>
+      <c r="B36" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36">
+        <v>1970</v>
+      </c>
+      <c r="D36" t="s">
+        <v>98</v>
+      </c>
+      <c r="E36" t="s">
+        <v>99</v>
+      </c>
+      <c r="F36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" t="s">
+        <v>55</v>
+      </c>
+      <c r="C37">
+        <v>1970</v>
+      </c>
+      <c r="D37" t="s">
+        <v>98</v>
+      </c>
+      <c r="E37" t="s">
+        <v>99</v>
+      </c>
+      <c r="F37" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>101</v>
+      </c>
+      <c r="B38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38">
+        <v>1970</v>
+      </c>
+      <c r="D38" t="s">
+        <v>98</v>
+      </c>
+      <c r="E38" t="s">
+        <v>99</v>
+      </c>
+      <c r="F38" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39">
+        <v>1970</v>
+      </c>
+      <c r="D39" t="s">
+        <v>98</v>
+      </c>
+      <c r="E39" t="s">
+        <v>99</v>
+      </c>
+      <c r="F39" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>101</v>
+      </c>
+      <c r="B40" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40">
+        <v>1970</v>
+      </c>
+      <c r="D40" t="s">
+        <v>98</v>
+      </c>
+      <c r="E40" t="s">
+        <v>99</v>
+      </c>
+      <c r="F40" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>101</v>
+      </c>
+      <c r="B41" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41">
+        <v>1970</v>
+      </c>
+      <c r="D41" t="s">
+        <v>98</v>
+      </c>
+      <c r="E41" t="s">
+        <v>99</v>
+      </c>
+      <c r="F41" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>115</v>
+      </c>
+      <c r="B42" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42">
+        <v>1970</v>
+      </c>
+      <c r="D42" t="s">
+        <v>98</v>
+      </c>
+      <c r="E42" t="s">
+        <v>99</v>
+      </c>
+      <c r="F42" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>115</v>
+      </c>
+      <c r="B43" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43">
+        <v>1970</v>
+      </c>
+      <c r="D43" t="s">
+        <v>98</v>
+      </c>
+      <c r="E43" t="s">
+        <v>99</v>
+      </c>
+      <c r="F43" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>115</v>
+      </c>
+      <c r="B44" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44">
+        <v>1970</v>
+      </c>
+      <c r="D44" t="s">
+        <v>98</v>
+      </c>
+      <c r="E44" t="s">
+        <v>99</v>
+      </c>
+      <c r="F44" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>115</v>
+      </c>
+      <c r="B45" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45">
+        <v>1970</v>
+      </c>
+      <c r="D45" t="s">
+        <v>98</v>
+      </c>
+      <c r="E45" t="s">
+        <v>99</v>
+      </c>
+      <c r="F45" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>116</v>
+      </c>
+      <c r="B46" t="s">
+        <v>65</v>
+      </c>
+      <c r="C46">
+        <v>1970</v>
+      </c>
+      <c r="D46" t="s">
+        <v>98</v>
+      </c>
+      <c r="E46" t="s">
+        <v>99</v>
+      </c>
+      <c r="F46" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
+        <v>116</v>
+      </c>
+      <c r="B47" t="s">
+        <v>84</v>
+      </c>
+      <c r="C47">
+        <v>1970</v>
+      </c>
+      <c r="D47" t="s">
+        <v>98</v>
+      </c>
+      <c r="E47" t="s">
+        <v>99</v>
+      </c>
+      <c r="F47" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
+        <v>117</v>
+      </c>
+      <c r="B48" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48">
+        <v>1970</v>
+      </c>
+      <c r="D48" t="s">
+        <v>98</v>
+      </c>
+      <c r="E48" t="s">
+        <v>99</v>
+      </c>
+      <c r="F48" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>117</v>
+      </c>
+      <c r="B49" t="s">
+        <v>84</v>
+      </c>
+      <c r="C49">
+        <v>1970</v>
+      </c>
+      <c r="D49" t="s">
+        <v>98</v>
+      </c>
+      <c r="E49" t="s">
+        <v>99</v>
+      </c>
+      <c r="F49" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>117</v>
+      </c>
+      <c r="B50" t="s">
+        <v>56</v>
+      </c>
+      <c r="C50">
+        <v>1970</v>
+      </c>
+      <c r="D50" t="s">
+        <v>98</v>
+      </c>
+      <c r="E50" t="s">
+        <v>99</v>
+      </c>
+      <c r="F50" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>117</v>
+      </c>
+      <c r="B51" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51">
+        <v>1970</v>
+      </c>
+      <c r="D51" t="s">
+        <v>98</v>
+      </c>
+      <c r="E51" t="s">
+        <v>99</v>
+      </c>
+      <c r="F51" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
+        <v>118</v>
+      </c>
+      <c r="B52" t="s">
+        <v>65</v>
+      </c>
+      <c r="C52">
+        <v>1970</v>
+      </c>
+      <c r="D52" t="s">
+        <v>98</v>
+      </c>
+      <c r="E52" t="s">
+        <v>99</v>
+      </c>
+      <c r="F52" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" t="s">
+        <v>118</v>
+      </c>
+      <c r="B53" t="s">
+        <v>84</v>
+      </c>
+      <c r="C53">
+        <v>1970</v>
+      </c>
+      <c r="D53" t="s">
+        <v>98</v>
+      </c>
+      <c r="E53" t="s">
+        <v>99</v>
+      </c>
+      <c r="F53" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" t="s">
+        <v>118</v>
+      </c>
+      <c r="B54" t="s">
+        <v>56</v>
+      </c>
+      <c r="C54">
+        <v>1970</v>
+      </c>
+      <c r="D54" t="s">
+        <v>98</v>
+      </c>
+      <c r="E54" t="s">
+        <v>99</v>
+      </c>
+      <c r="F54" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" t="s">
+        <v>118</v>
+      </c>
+      <c r="B55" t="s">
+        <v>55</v>
+      </c>
+      <c r="C55">
+        <v>1970</v>
+      </c>
+      <c r="D55" t="s">
+        <v>98</v>
+      </c>
+      <c r="E55" t="s">
+        <v>99</v>
+      </c>
+      <c r="F55" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" t="s">
+        <v>119</v>
+      </c>
+      <c r="B56" t="s">
+        <v>65</v>
+      </c>
+      <c r="C56">
+        <v>1970</v>
+      </c>
+      <c r="D56" t="s">
+        <v>98</v>
+      </c>
+      <c r="E56" t="s">
+        <v>99</v>
+      </c>
+      <c r="F56" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" t="s">
+        <v>119</v>
+      </c>
+      <c r="B57" t="s">
+        <v>84</v>
+      </c>
+      <c r="C57">
+        <v>1970</v>
+      </c>
+      <c r="D57" t="s">
+        <v>98</v>
+      </c>
+      <c r="E57" t="s">
+        <v>99</v>
+      </c>
+      <c r="F57" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" t="s">
+        <v>119</v>
+      </c>
+      <c r="B58" t="s">
+        <v>56</v>
+      </c>
+      <c r="C58">
+        <v>1970</v>
+      </c>
+      <c r="D58" t="s">
+        <v>98</v>
+      </c>
+      <c r="E58" t="s">
+        <v>99</v>
+      </c>
+      <c r="F58" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" t="s">
+        <v>119</v>
+      </c>
+      <c r="B59" t="s">
+        <v>55</v>
+      </c>
+      <c r="C59">
+        <v>1970</v>
+      </c>
+      <c r="D59" t="s">
+        <v>98</v>
+      </c>
+      <c r="E59" t="s">
+        <v>99</v>
+      </c>
+      <c r="F59" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" t="s">
+        <v>120</v>
+      </c>
+      <c r="B60" t="s">
+        <v>65</v>
+      </c>
+      <c r="C60">
+        <v>1970</v>
+      </c>
+      <c r="D60" t="s">
+        <v>98</v>
+      </c>
+      <c r="E60" t="s">
+        <v>99</v>
+      </c>
+      <c r="F60" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" t="s">
+        <v>120</v>
+      </c>
+      <c r="B61" t="s">
+        <v>84</v>
+      </c>
+      <c r="C61">
+        <v>1970</v>
+      </c>
+      <c r="D61" t="s">
+        <v>98</v>
+      </c>
+      <c r="E61" t="s">
+        <v>99</v>
+      </c>
+      <c r="F61" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" t="s">
+        <v>120</v>
+      </c>
+      <c r="B62" t="s">
+        <v>56</v>
+      </c>
+      <c r="C62">
+        <v>1970</v>
+      </c>
+      <c r="D62" t="s">
+        <v>98</v>
+      </c>
+      <c r="E62" t="s">
+        <v>99</v>
+      </c>
+      <c r="F62" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" t="s">
+        <v>120</v>
+      </c>
+      <c r="B63" t="s">
+        <v>55</v>
+      </c>
+      <c r="C63">
+        <v>1970</v>
+      </c>
+      <c r="D63" t="s">
+        <v>98</v>
+      </c>
+      <c r="E63" t="s">
+        <v>99</v>
+      </c>
+      <c r="F63" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" t="s">
+        <v>121</v>
+      </c>
+      <c r="B64" t="s">
+        <v>65</v>
+      </c>
+      <c r="C64">
+        <v>1970</v>
+      </c>
+      <c r="D64" t="s">
+        <v>98</v>
+      </c>
+      <c r="E64" t="s">
+        <v>99</v>
+      </c>
+      <c r="F64" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" t="s">
+        <v>121</v>
+      </c>
+      <c r="B65" t="s">
+        <v>84</v>
+      </c>
+      <c r="C65">
+        <v>1970</v>
+      </c>
+      <c r="D65" t="s">
+        <v>98</v>
+      </c>
+      <c r="E65" t="s">
+        <v>99</v>
+      </c>
+      <c r="F65" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" t="s">
+        <v>121</v>
+      </c>
+      <c r="B66" t="s">
+        <v>56</v>
+      </c>
+      <c r="C66">
+        <v>1970</v>
+      </c>
+      <c r="D66" t="s">
+        <v>98</v>
+      </c>
+      <c r="E66" t="s">
+        <v>99</v>
+      </c>
+      <c r="F66" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" t="s">
+        <v>121</v>
+      </c>
+      <c r="B67" t="s">
+        <v>55</v>
+      </c>
+      <c r="C67">
+        <v>1970</v>
+      </c>
+      <c r="D67" t="s">
+        <v>98</v>
+      </c>
+      <c r="E67" t="s">
+        <v>99</v>
+      </c>
+      <c r="F67" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" t="s">
+        <v>122</v>
+      </c>
+      <c r="B68" t="s">
+        <v>65</v>
+      </c>
+      <c r="C68">
+        <v>1970</v>
+      </c>
+      <c r="D68" t="s">
+        <v>98</v>
+      </c>
+      <c r="E68" t="s">
+        <v>99</v>
+      </c>
+      <c r="F68" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" t="s">
+        <v>122</v>
+      </c>
+      <c r="B69" t="s">
+        <v>84</v>
+      </c>
+      <c r="C69">
+        <v>1970</v>
+      </c>
+      <c r="D69" t="s">
+        <v>98</v>
+      </c>
+      <c r="E69" t="s">
+        <v>99</v>
+      </c>
+      <c r="F69" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" t="s">
+        <v>122</v>
+      </c>
+      <c r="B70" t="s">
+        <v>56</v>
+      </c>
+      <c r="C70">
+        <v>1970</v>
+      </c>
+      <c r="D70" t="s">
+        <v>98</v>
+      </c>
+      <c r="E70" t="s">
+        <v>99</v>
+      </c>
+      <c r="F70" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" t="s">
+        <v>122</v>
+      </c>
+      <c r="B71" t="s">
+        <v>55</v>
+      </c>
+      <c r="C71">
+        <v>1970</v>
+      </c>
+      <c r="D71" t="s">
+        <v>98</v>
+      </c>
+      <c r="E71" t="s">
+        <v>99</v>
+      </c>
+      <c r="F71" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" t="s">
+        <v>103</v>
+      </c>
+      <c r="B72" t="s">
+        <v>65</v>
+      </c>
+      <c r="C72">
+        <v>1970</v>
+      </c>
+      <c r="D72" t="s">
+        <v>98</v>
+      </c>
+      <c r="E72" t="s">
+        <v>99</v>
+      </c>
+      <c r="F72" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" t="s">
+        <v>103</v>
+      </c>
+      <c r="B73" t="s">
+        <v>84</v>
+      </c>
+      <c r="C73">
+        <v>1970</v>
+      </c>
+      <c r="D73" t="s">
+        <v>98</v>
+      </c>
+      <c r="E73" t="s">
+        <v>99</v>
+      </c>
+      <c r="F73" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" t="s">
+        <v>103</v>
+      </c>
+      <c r="B74" t="s">
+        <v>56</v>
+      </c>
+      <c r="C74">
+        <v>1970</v>
+      </c>
+      <c r="D74" t="s">
+        <v>98</v>
+      </c>
+      <c r="E74" t="s">
+        <v>99</v>
+      </c>
+      <c r="F74" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" t="s">
+        <v>103</v>
+      </c>
+      <c r="B75" t="s">
+        <v>55</v>
+      </c>
+      <c r="C75">
+        <v>1970</v>
+      </c>
+      <c r="D75" t="s">
+        <v>98</v>
+      </c>
+      <c r="E75" t="s">
+        <v>99</v>
+      </c>
+      <c r="F75" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" t="s">
+        <v>123</v>
+      </c>
+      <c r="B76" t="s">
+        <v>65</v>
+      </c>
+      <c r="C76">
+        <v>1970</v>
+      </c>
+      <c r="D76" t="s">
+        <v>98</v>
+      </c>
+      <c r="E76" t="s">
+        <v>99</v>
+      </c>
+      <c r="F76" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" t="s">
+        <v>123</v>
+      </c>
+      <c r="B77" t="s">
+        <v>84</v>
+      </c>
+      <c r="C77">
+        <v>1970</v>
+      </c>
+      <c r="D77" t="s">
+        <v>98</v>
+      </c>
+      <c r="E77" t="s">
+        <v>99</v>
+      </c>
+      <c r="F77" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" t="s">
+        <v>123</v>
+      </c>
+      <c r="B78" t="s">
+        <v>56</v>
+      </c>
+      <c r="C78">
+        <v>1970</v>
+      </c>
+      <c r="D78" t="s">
+        <v>98</v>
+      </c>
+      <c r="E78" t="s">
+        <v>99</v>
+      </c>
+      <c r="F78" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" t="s">
+        <v>123</v>
+      </c>
+      <c r="B79" t="s">
+        <v>55</v>
+      </c>
+      <c r="C79">
+        <v>1970</v>
+      </c>
+      <c r="D79" t="s">
+        <v>98</v>
+      </c>
+      <c r="E79" t="s">
+        <v>99</v>
+      </c>
+      <c r="F79" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" t="s">
+        <v>94</v>
+      </c>
+      <c r="B80" t="s">
+        <v>65</v>
+      </c>
+      <c r="C80">
+        <v>1970</v>
+      </c>
+      <c r="D80" t="s">
+        <v>98</v>
+      </c>
+      <c r="E80" t="s">
+        <v>99</v>
+      </c>
+      <c r="F80" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" t="s">
+        <v>94</v>
+      </c>
+      <c r="B81" t="s">
+        <v>84</v>
+      </c>
+      <c r="C81">
+        <v>1970</v>
+      </c>
+      <c r="D81" t="s">
+        <v>98</v>
+      </c>
+      <c r="E81" t="s">
+        <v>99</v>
+      </c>
+      <c r="F81" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" t="s">
+        <v>94</v>
+      </c>
+      <c r="B82" t="s">
+        <v>56</v>
+      </c>
+      <c r="C82">
+        <v>1970</v>
+      </c>
+      <c r="D82" t="s">
+        <v>98</v>
+      </c>
+      <c r="E82" t="s">
+        <v>99</v>
+      </c>
+      <c r="F82" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" t="s">
+        <v>94</v>
+      </c>
+      <c r="B83" t="s">
+        <v>55</v>
+      </c>
+      <c r="C83">
+        <v>1970</v>
+      </c>
+      <c r="D83" t="s">
+        <v>98</v>
+      </c>
+      <c r="E83" t="s">
+        <v>99</v>
+      </c>
+      <c r="F83" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" t="s">
+        <v>124</v>
+      </c>
+      <c r="B84" t="s">
+        <v>65</v>
+      </c>
+      <c r="C84">
+        <v>1970</v>
+      </c>
+      <c r="D84" t="s">
+        <v>98</v>
+      </c>
+      <c r="E84" t="s">
+        <v>99</v>
+      </c>
+      <c r="F84" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" t="s">
+        <v>124</v>
+      </c>
+      <c r="B85" t="s">
+        <v>84</v>
+      </c>
+      <c r="C85">
+        <v>1970</v>
+      </c>
+      <c r="D85" t="s">
+        <v>98</v>
+      </c>
+      <c r="E85" t="s">
+        <v>99</v>
+      </c>
+      <c r="F85" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" t="s">
+        <v>124</v>
+      </c>
+      <c r="B86" t="s">
+        <v>56</v>
+      </c>
+      <c r="C86">
+        <v>1970</v>
+      </c>
+      <c r="D86" t="s">
+        <v>98</v>
+      </c>
+      <c r="E86" t="s">
+        <v>99</v>
+      </c>
+      <c r="F86" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" t="s">
+        <v>124</v>
+      </c>
+      <c r="B87" t="s">
+        <v>55</v>
+      </c>
+      <c r="C87">
+        <v>1970</v>
+      </c>
+      <c r="D87" t="s">
+        <v>98</v>
+      </c>
+      <c r="E87" t="s">
+        <v>99</v>
+      </c>
+      <c r="F87" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" t="s">
+        <v>125</v>
+      </c>
+      <c r="B88" t="s">
+        <v>84</v>
+      </c>
+      <c r="C88">
+        <v>1970</v>
+      </c>
+      <c r="D88" t="s">
+        <v>98</v>
+      </c>
+      <c r="E88" t="s">
+        <v>99</v>
+      </c>
+      <c r="F88" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" t="s">
+        <v>126</v>
+      </c>
+      <c r="B89" t="s">
+        <v>65</v>
+      </c>
+      <c r="C89">
+        <v>1970</v>
+      </c>
+      <c r="D89" t="s">
+        <v>98</v>
+      </c>
+      <c r="E89" t="s">
+        <v>99</v>
+      </c>
+      <c r="F89" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" t="s">
+        <v>126</v>
+      </c>
+      <c r="B90" t="s">
+        <v>84</v>
+      </c>
+      <c r="C90">
+        <v>1970</v>
+      </c>
+      <c r="D90" t="s">
+        <v>98</v>
+      </c>
+      <c r="E90" t="s">
+        <v>99</v>
+      </c>
+      <c r="F90" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" t="s">
+        <v>126</v>
+      </c>
+      <c r="B91" t="s">
+        <v>56</v>
+      </c>
+      <c r="C91">
+        <v>1970</v>
+      </c>
+      <c r="D91" t="s">
+        <v>98</v>
+      </c>
+      <c r="E91" t="s">
+        <v>99</v>
+      </c>
+      <c r="F91" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" t="s">
+        <v>126</v>
+      </c>
+      <c r="B92" t="s">
+        <v>55</v>
+      </c>
+      <c r="C92">
+        <v>1970</v>
+      </c>
+      <c r="D92" t="s">
+        <v>98</v>
+      </c>
+      <c r="E92" t="s">
+        <v>99</v>
+      </c>
+      <c r="F92" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" t="s">
+        <v>127</v>
+      </c>
+      <c r="B93" t="s">
+        <v>65</v>
+      </c>
+      <c r="C93">
+        <v>1970</v>
+      </c>
+      <c r="D93" t="s">
+        <v>98</v>
+      </c>
+      <c r="E93" t="s">
+        <v>99</v>
+      </c>
+      <c r="F93" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" t="s">
+        <v>127</v>
+      </c>
+      <c r="B94" t="s">
+        <v>84</v>
+      </c>
+      <c r="C94">
+        <v>1970</v>
+      </c>
+      <c r="D94" t="s">
+        <v>98</v>
+      </c>
+      <c r="E94" t="s">
+        <v>99</v>
+      </c>
+      <c r="F94" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" t="s">
+        <v>127</v>
+      </c>
+      <c r="B95" t="s">
+        <v>56</v>
+      </c>
+      <c r="C95">
+        <v>1970</v>
+      </c>
+      <c r="D95" t="s">
+        <v>98</v>
+      </c>
+      <c r="E95" t="s">
+        <v>99</v>
+      </c>
+      <c r="F95" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" t="s">
+        <v>127</v>
+      </c>
+      <c r="B96" t="s">
+        <v>55</v>
+      </c>
+      <c r="C96">
+        <v>1970</v>
+      </c>
+      <c r="D96" t="s">
+        <v>98</v>
+      </c>
+      <c r="E96" t="s">
+        <v>99</v>
+      </c>
+      <c r="F96" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97" t="s">
+        <v>128</v>
+      </c>
+      <c r="B97" t="s">
+        <v>65</v>
+      </c>
+      <c r="C97">
+        <v>1970</v>
+      </c>
+      <c r="D97" t="s">
+        <v>98</v>
+      </c>
+      <c r="E97" t="s">
+        <v>99</v>
+      </c>
+      <c r="F97" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" t="s">
+        <v>128</v>
+      </c>
+      <c r="B98" t="s">
+        <v>84</v>
+      </c>
+      <c r="C98">
+        <v>1970</v>
+      </c>
+      <c r="D98" t="s">
+        <v>98</v>
+      </c>
+      <c r="E98" t="s">
+        <v>99</v>
+      </c>
+      <c r="F98" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" t="s">
+        <v>128</v>
+      </c>
+      <c r="B99" t="s">
+        <v>56</v>
+      </c>
+      <c r="C99">
+        <v>1970</v>
+      </c>
+      <c r="D99" t="s">
+        <v>98</v>
+      </c>
+      <c r="E99" t="s">
+        <v>99</v>
+      </c>
+      <c r="F99" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100" t="s">
+        <v>128</v>
+      </c>
+      <c r="B100" t="s">
+        <v>55</v>
+      </c>
+      <c r="C100">
+        <v>1970</v>
+      </c>
+      <c r="D100" t="s">
+        <v>98</v>
+      </c>
+      <c r="E100" t="s">
+        <v>99</v>
+      </c>
+      <c r="F100" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101" t="s">
+        <v>129</v>
+      </c>
+      <c r="B101" t="s">
+        <v>65</v>
+      </c>
+      <c r="C101">
+        <v>1970</v>
+      </c>
+      <c r="D101" t="s">
+        <v>98</v>
+      </c>
+      <c r="E101" t="s">
+        <v>99</v>
+      </c>
+      <c r="F101" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="A102" t="s">
+        <v>129</v>
+      </c>
+      <c r="B102" t="s">
+        <v>84</v>
+      </c>
+      <c r="C102">
+        <v>1970</v>
+      </c>
+      <c r="D102" t="s">
+        <v>98</v>
+      </c>
+      <c r="E102" t="s">
+        <v>99</v>
+      </c>
+      <c r="F102" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
+      <c r="A103" t="s">
+        <v>129</v>
+      </c>
+      <c r="B103" t="s">
+        <v>56</v>
+      </c>
+      <c r="C103">
+        <v>1970</v>
+      </c>
+      <c r="D103" t="s">
+        <v>98</v>
+      </c>
+      <c r="E103" t="s">
+        <v>99</v>
+      </c>
+      <c r="F103" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104" t="s">
+        <v>129</v>
+      </c>
+      <c r="B104" t="s">
+        <v>55</v>
+      </c>
+      <c r="C104">
+        <v>1970</v>
+      </c>
+      <c r="D104" t="s">
+        <v>98</v>
+      </c>
+      <c r="E104" t="s">
+        <v>99</v>
+      </c>
+      <c r="F104" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105" t="s">
+        <v>130</v>
+      </c>
+      <c r="B105" t="s">
+        <v>65</v>
+      </c>
+      <c r="C105">
+        <v>1970</v>
+      </c>
+      <c r="D105" t="s">
+        <v>98</v>
+      </c>
+      <c r="E105" t="s">
+        <v>99</v>
+      </c>
+      <c r="F105" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106" t="s">
+        <v>130</v>
+      </c>
+      <c r="B106" t="s">
+        <v>84</v>
+      </c>
+      <c r="C106">
+        <v>1970</v>
+      </c>
+      <c r="D106" t="s">
+        <v>98</v>
+      </c>
+      <c r="E106" t="s">
+        <v>99</v>
+      </c>
+      <c r="F106" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107" t="s">
+        <v>130</v>
+      </c>
+      <c r="B107" t="s">
+        <v>56</v>
+      </c>
+      <c r="C107">
+        <v>1970</v>
+      </c>
+      <c r="D107" t="s">
+        <v>98</v>
+      </c>
+      <c r="E107" t="s">
+        <v>99</v>
+      </c>
+      <c r="F107" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108" t="s">
+        <v>130</v>
+      </c>
+      <c r="B108" t="s">
+        <v>55</v>
+      </c>
+      <c r="C108">
+        <v>1970</v>
+      </c>
+      <c r="D108" t="s">
+        <v>98</v>
+      </c>
+      <c r="E108" t="s">
+        <v>99</v>
+      </c>
+      <c r="F108" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2224,15 +4382,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2258,7 +4416,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>94</v>
       </c>
@@ -2282,6 +4440,64 @@
       </c>
       <c r="H2" t="s">
         <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>1982</v>
+      </c>
+      <c r="G3">
+        <v>2020</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>1990</v>
+      </c>
+      <c r="G4">
+        <v>2020</v>
+      </c>
+      <c r="H4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revise EMEP SO2 scaling
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/EMEP_NFR09_scaling_mapping_SO2.xlsx
+++ b/input/mappings/scaling/EMEP_NFR09_scaling_mapping_SO2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="0" windowWidth="24400" windowHeight="13680" tabRatio="500"/>
+    <workbookView xWindow="4180" yWindow="0" windowWidth="24400" windowHeight="13680" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="132">
   <si>
     <t>pre_ext_method</t>
   </si>
@@ -411,6 +411,12 @@
   </si>
   <si>
     <t>swe</t>
+  </si>
+  <si>
+    <t>svn</t>
+  </si>
+  <si>
+    <t>Don't scale prior to 1990 since we do not have consistent driver data at this level</t>
   </si>
 </sst>
 </file>
@@ -466,8 +472,54 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="243">
+  <cellStyleXfs count="289">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -718,7 +770,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="243">
+  <cellStyles count="289">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -840,6 +892,29 @@
     <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -961,6 +1036,29 @@
     <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1297,7 +1395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
@@ -2187,10 +2285,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G108"/>
+  <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93"/>
+    <sheetView topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70:C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2271,7 +2369,7 @@
         <v>56</v>
       </c>
       <c r="C4">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D4" t="s">
         <v>97</v>
@@ -2291,7 +2389,7 @@
         <v>55</v>
       </c>
       <c r="C5">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D5" t="s">
         <v>97</v>
@@ -2351,7 +2449,7 @@
         <v>56</v>
       </c>
       <c r="C8">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D8" t="s">
         <v>97</v>
@@ -2371,7 +2469,7 @@
         <v>55</v>
       </c>
       <c r="C9">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D9" t="s">
         <v>97</v>
@@ -2431,7 +2529,7 @@
         <v>56</v>
       </c>
       <c r="C12">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D12" t="s">
         <v>97</v>
@@ -2451,7 +2549,7 @@
         <v>55</v>
       </c>
       <c r="C13">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D13" t="s">
         <v>97</v>
@@ -2511,7 +2609,7 @@
         <v>56</v>
       </c>
       <c r="C16">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D16" t="s">
         <v>97</v>
@@ -2531,7 +2629,7 @@
         <v>55</v>
       </c>
       <c r="C17">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D17" t="s">
         <v>97</v>
@@ -2545,13 +2643,13 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B18" t="s">
         <v>64</v>
       </c>
       <c r="C18">
-        <v>1990</v>
+        <v>1970</v>
       </c>
       <c r="D18" t="s">
         <v>97</v>
@@ -2565,13 +2663,13 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B19" t="s">
         <v>83</v>
       </c>
       <c r="C19">
-        <v>1990</v>
+        <v>1970</v>
       </c>
       <c r="D19" t="s">
         <v>97</v>
@@ -2585,13 +2683,13 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B20" t="s">
         <v>56</v>
       </c>
       <c r="C20">
-        <v>1990</v>
+        <v>1980</v>
       </c>
       <c r="D20" t="s">
         <v>97</v>
@@ -2605,13 +2703,13 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B21" t="s">
         <v>55</v>
       </c>
       <c r="C21">
-        <v>1990</v>
+        <v>1980</v>
       </c>
       <c r="D21" t="s">
         <v>97</v>
@@ -2625,7 +2723,7 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B22" t="s">
         <v>64</v>
@@ -2645,7 +2743,7 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B23" t="s">
         <v>83</v>
@@ -2665,13 +2763,13 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B24" t="s">
         <v>56</v>
       </c>
       <c r="C24">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D24" t="s">
         <v>97</v>
@@ -2685,13 +2783,13 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B25" t="s">
         <v>55</v>
       </c>
       <c r="C25">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D25" t="s">
         <v>97</v>
@@ -2705,7 +2803,7 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B26" t="s">
         <v>64</v>
@@ -2725,7 +2823,7 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B27" t="s">
         <v>83</v>
@@ -2745,13 +2843,13 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B28" t="s">
         <v>56</v>
       </c>
       <c r="C28">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D28" t="s">
         <v>97</v>
@@ -2765,13 +2863,13 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B29" t="s">
         <v>55</v>
       </c>
       <c r="C29">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D29" t="s">
         <v>97</v>
@@ -2785,7 +2883,7 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B30" t="s">
         <v>64</v>
@@ -2805,7 +2903,7 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B31" t="s">
         <v>83</v>
@@ -2825,13 +2923,13 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B32" t="s">
         <v>56</v>
       </c>
       <c r="C32">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D32" t="s">
         <v>97</v>
@@ -2845,13 +2943,13 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B33" t="s">
         <v>55</v>
       </c>
       <c r="C33">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D33" t="s">
         <v>97</v>
@@ -2865,7 +2963,7 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B34" t="s">
         <v>64</v>
@@ -2885,7 +2983,7 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B35" t="s">
         <v>83</v>
@@ -2905,13 +3003,13 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B36" t="s">
         <v>56</v>
       </c>
       <c r="C36">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D36" t="s">
         <v>97</v>
@@ -2925,13 +3023,13 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B37" t="s">
         <v>55</v>
       </c>
       <c r="C37">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D37" t="s">
         <v>97</v>
@@ -2945,7 +3043,7 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="B38" t="s">
         <v>64</v>
@@ -2965,7 +3063,7 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="B39" t="s">
         <v>83</v>
@@ -2985,10 +3083,10 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="B40" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C40">
         <v>1970</v>
@@ -3005,10 +3103,10 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="B41" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="C41">
         <v>1970</v>
@@ -3025,13 +3123,13 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B42" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C42">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D42" t="s">
         <v>97</v>
@@ -3045,13 +3143,13 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B43" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="C43">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D43" t="s">
         <v>97</v>
@@ -3065,10 +3163,10 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B44" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C44">
         <v>1970</v>
@@ -3085,10 +3183,10 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B45" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="C45">
         <v>1970</v>
@@ -3105,13 +3203,13 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B46" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C46">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D46" t="s">
         <v>97</v>
@@ -3125,13 +3223,13 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B47" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="C47">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D47" t="s">
         <v>97</v>
@@ -3145,7 +3243,7 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B48" t="s">
         <v>64</v>
@@ -3165,7 +3263,7 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B49" t="s">
         <v>83</v>
@@ -3185,13 +3283,13 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B50" t="s">
         <v>56</v>
       </c>
       <c r="C50">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D50" t="s">
         <v>97</v>
@@ -3205,13 +3303,13 @@
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B51" t="s">
         <v>55</v>
       </c>
       <c r="C51">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D51" t="s">
         <v>97</v>
@@ -3225,7 +3323,7 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="B52" t="s">
         <v>64</v>
@@ -3245,7 +3343,7 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="B53" t="s">
         <v>83</v>
@@ -3265,13 +3363,13 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="B54" t="s">
         <v>56</v>
       </c>
       <c r="C54">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D54" t="s">
         <v>97</v>
@@ -3285,13 +3383,13 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="B55" t="s">
         <v>55</v>
       </c>
       <c r="C55">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D55" t="s">
         <v>97</v>
@@ -3305,7 +3403,7 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B56" t="s">
         <v>64</v>
@@ -3325,7 +3423,7 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B57" t="s">
         <v>83</v>
@@ -3345,13 +3443,13 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B58" t="s">
         <v>56</v>
       </c>
       <c r="C58">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D58" t="s">
         <v>97</v>
@@ -3365,13 +3463,13 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B59" t="s">
         <v>55</v>
       </c>
       <c r="C59">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D59" t="s">
         <v>97</v>
@@ -3385,13 +3483,13 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="B60" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="C60">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D60" t="s">
         <v>97</v>
@@ -3405,10 +3503,10 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="B61" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="C61">
         <v>1970</v>
@@ -3425,10 +3523,10 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="B62" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="C62">
         <v>1970</v>
@@ -3445,13 +3543,13 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="B63" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C63">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D63" t="s">
         <v>97</v>
@@ -3465,13 +3563,13 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B64" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C64">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D64" t="s">
         <v>97</v>
@@ -3485,10 +3583,10 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="B65" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="C65">
         <v>1970</v>
@@ -3505,10 +3603,10 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="B66" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="C66">
         <v>1970</v>
@@ -3525,13 +3623,13 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="B67" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C67">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D67" t="s">
         <v>97</v>
@@ -3545,13 +3643,13 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B68" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C68">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D68" t="s">
         <v>97</v>
@@ -3560,38 +3658,18 @@
         <v>98</v>
       </c>
       <c r="F68" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
-      <c r="A69" t="s">
-        <v>121</v>
-      </c>
-      <c r="B69" t="s">
-        <v>83</v>
-      </c>
-      <c r="C69">
-        <v>1970</v>
-      </c>
-      <c r="D69" t="s">
-        <v>97</v>
-      </c>
-      <c r="E69" t="s">
-        <v>98</v>
-      </c>
-      <c r="F69" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B70" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C70">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D70" t="s">
         <v>97</v>
@@ -3605,13 +3683,13 @@
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B71" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="C71">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D71" t="s">
         <v>97</v>
@@ -3625,13 +3703,13 @@
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="B72" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C72">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="D72" t="s">
         <v>97</v>
@@ -3645,13 +3723,13 @@
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="B73" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="C73">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="D73" t="s">
         <v>97</v>
@@ -3665,13 +3743,13 @@
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="B74" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C74">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D74" t="s">
         <v>97</v>
@@ -3685,13 +3763,13 @@
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="B75" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="C75">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D75" t="s">
         <v>97</v>
@@ -3705,13 +3783,13 @@
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B76" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C76">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="D76" t="s">
         <v>97</v>
@@ -3725,13 +3803,13 @@
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B77" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="C77">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="D77" t="s">
         <v>97</v>
@@ -3748,10 +3826,10 @@
         <v>122</v>
       </c>
       <c r="B78" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C78">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D78" t="s">
         <v>97</v>
@@ -3768,10 +3846,10 @@
         <v>122</v>
       </c>
       <c r="B79" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="C79">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D79" t="s">
         <v>97</v>
@@ -3785,13 +3863,13 @@
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>93</v>
+        <v>122</v>
       </c>
       <c r="B80" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C80">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="D80" t="s">
         <v>97</v>
@@ -3805,13 +3883,13 @@
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>93</v>
+        <v>122</v>
       </c>
       <c r="B81" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="C81">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="D81" t="s">
         <v>97</v>
@@ -3825,13 +3903,13 @@
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>93</v>
+        <v>116</v>
       </c>
       <c r="B82" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C82">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D82" t="s">
         <v>97</v>
@@ -3845,13 +3923,13 @@
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>93</v>
+        <v>116</v>
       </c>
       <c r="B83" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="C83">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="D83" t="s">
         <v>97</v>
@@ -3865,13 +3943,13 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B84" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C84">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="D84" t="s">
         <v>97</v>
@@ -3885,13 +3963,13 @@
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B85" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="C85">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="D85" t="s">
         <v>97</v>
@@ -3900,38 +3978,18 @@
         <v>98</v>
       </c>
       <c r="F85" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6">
-      <c r="A86" t="s">
-        <v>123</v>
-      </c>
-      <c r="B86" t="s">
-        <v>56</v>
-      </c>
-      <c r="C86">
-        <v>1970</v>
-      </c>
-      <c r="D86" t="s">
-        <v>97</v>
-      </c>
-      <c r="E86" t="s">
-        <v>98</v>
-      </c>
-      <c r="F86" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B87" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C87">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="D87" t="s">
         <v>97</v>
@@ -3945,13 +4003,13 @@
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B88" t="s">
         <v>83</v>
       </c>
       <c r="C88">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="D88" t="s">
         <v>97</v>
@@ -3965,13 +4023,13 @@
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B89" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C89">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="D89" t="s">
         <v>97</v>
@@ -3985,13 +4043,13 @@
     </row>
     <row r="90" spans="1:6">
       <c r="A90" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B90" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="C90">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="D90" t="s">
         <v>97</v>
@@ -4008,10 +4066,10 @@
         <v>125</v>
       </c>
       <c r="B91" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C91">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="D91" t="s">
         <v>97</v>
@@ -4028,10 +4086,10 @@
         <v>125</v>
       </c>
       <c r="B92" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="C92">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="D92" t="s">
         <v>97</v>
@@ -4045,13 +4103,13 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B93" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C93">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="D93" t="s">
         <v>97</v>
@@ -4065,13 +4123,13 @@
     </row>
     <row r="94" spans="1:6">
       <c r="A94" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B94" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="C94">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="D94" t="s">
         <v>97</v>
@@ -4080,38 +4138,18 @@
         <v>98</v>
       </c>
       <c r="F94" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6">
-      <c r="A95" t="s">
-        <v>126</v>
-      </c>
-      <c r="B95" t="s">
-        <v>56</v>
-      </c>
-      <c r="C95">
-        <v>1970</v>
-      </c>
-      <c r="D95" t="s">
-        <v>97</v>
-      </c>
-      <c r="E95" t="s">
-        <v>98</v>
-      </c>
-      <c r="F95" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B96" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C96">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="D96" t="s">
         <v>97</v>
@@ -4125,13 +4163,13 @@
     </row>
     <row r="97" spans="1:6">
       <c r="A97" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B97" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="C97">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="D97" t="s">
         <v>97</v>
@@ -4145,13 +4183,13 @@
     </row>
     <row r="98" spans="1:6">
       <c r="A98" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B98" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="C98">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="D98" t="s">
         <v>97</v>
@@ -4165,13 +4203,13 @@
     </row>
     <row r="99" spans="1:6">
       <c r="A99" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B99" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C99">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="D99" t="s">
         <v>97</v>
@@ -4185,13 +4223,13 @@
     </row>
     <row r="100" spans="1:6">
       <c r="A100" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="B100" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C100">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="D100" t="s">
         <v>97</v>
@@ -4205,13 +4243,13 @@
     </row>
     <row r="101" spans="1:6">
       <c r="A101" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="B101" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="C101">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="D101" t="s">
         <v>97</v>
@@ -4225,13 +4263,13 @@
     </row>
     <row r="102" spans="1:6">
       <c r="A102" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="B102" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="C102">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="D102" t="s">
         <v>97</v>
@@ -4245,13 +4283,13 @@
     </row>
     <row r="103" spans="1:6">
       <c r="A103" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="B103" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C103">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="D103" t="s">
         <v>97</v>
@@ -4268,10 +4306,10 @@
         <v>128</v>
       </c>
       <c r="B104" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C104">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="D104" t="s">
         <v>97</v>
@@ -4285,13 +4323,13 @@
     </row>
     <row r="105" spans="1:6">
       <c r="A105" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B105" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="C105">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="D105" t="s">
         <v>97</v>
@@ -4305,13 +4343,13 @@
     </row>
     <row r="106" spans="1:6">
       <c r="A106" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B106" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="C106">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="D106" t="s">
         <v>97</v>
@@ -4325,13 +4363,13 @@
     </row>
     <row r="107" spans="1:6">
       <c r="A107" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B107" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C107">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="D107" t="s">
         <v>97</v>
@@ -4345,21 +4383,81 @@
     </row>
     <row r="108" spans="1:6">
       <c r="A108" t="s">
-        <v>129</v>
+        <v>93</v>
       </c>
       <c r="B108" t="s">
+        <v>64</v>
+      </c>
+      <c r="C108">
+        <v>1990</v>
+      </c>
+      <c r="D108" t="s">
+        <v>97</v>
+      </c>
+      <c r="E108" t="s">
+        <v>98</v>
+      </c>
+      <c r="F108" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109" t="s">
+        <v>93</v>
+      </c>
+      <c r="B109" t="s">
+        <v>83</v>
+      </c>
+      <c r="C109">
+        <v>1990</v>
+      </c>
+      <c r="D109" t="s">
+        <v>97</v>
+      </c>
+      <c r="E109" t="s">
+        <v>98</v>
+      </c>
+      <c r="F109" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="A110" t="s">
+        <v>93</v>
+      </c>
+      <c r="B110" t="s">
+        <v>56</v>
+      </c>
+      <c r="C110">
+        <v>1990</v>
+      </c>
+      <c r="D110" t="s">
+        <v>97</v>
+      </c>
+      <c r="E110" t="s">
+        <v>98</v>
+      </c>
+      <c r="F110" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111" t="s">
+        <v>93</v>
+      </c>
+      <c r="B111" t="s">
         <v>55</v>
       </c>
-      <c r="C108">
-        <v>1970</v>
-      </c>
-      <c r="D108" t="s">
-        <v>97</v>
-      </c>
-      <c r="E108" t="s">
-        <v>98</v>
-      </c>
-      <c r="F108" t="s">
+      <c r="C111">
+        <v>1990</v>
+      </c>
+      <c r="D111" t="s">
+        <v>97</v>
+      </c>
+      <c r="E111" t="s">
+        <v>98</v>
+      </c>
+      <c r="F111" t="s">
         <v>99</v>
       </c>
     </row>
@@ -4376,10 +4474,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4430,7 +4528,7 @@
         <v>1990</v>
       </c>
       <c r="G2">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="H2" t="s">
         <v>95</v>
@@ -4492,6 +4590,32 @@
       </c>
       <c r="I4" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>1990</v>
+      </c>
+      <c r="G5">
+        <v>2020</v>
+      </c>
+      <c r="H5" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated S scaling to improve match to inventory data in 1980 and before.
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/EMEP_NFR09_scaling_mapping_SO2.xlsx
+++ b/input/mappings/scaling/EMEP_NFR09_scaling_mapping_SO2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4180" yWindow="0" windowWidth="24400" windowHeight="13680" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="14400" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
@@ -2287,8 +2287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70:C74"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="K102" sqref="K102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2849,10 +2849,10 @@
         <v>56</v>
       </c>
       <c r="C28">
-        <v>1980</v>
+        <v>1990</v>
       </c>
       <c r="D28" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E28" t="s">
         <v>98</v>
@@ -2869,10 +2869,10 @@
         <v>55</v>
       </c>
       <c r="C29">
-        <v>1980</v>
+        <v>1990</v>
       </c>
       <c r="D29" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E29" t="s">
         <v>98</v>
@@ -4192,7 +4192,7 @@
         <v>1990</v>
       </c>
       <c r="D98" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E98" t="s">
         <v>98</v>
@@ -4212,7 +4212,7 @@
         <v>1990</v>
       </c>
       <c r="D99" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E99" t="s">
         <v>98</v>
@@ -4432,7 +4432,7 @@
         <v>1990</v>
       </c>
       <c r="D110" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E110" t="s">
         <v>98</v>
@@ -4452,7 +4452,7 @@
         <v>1990</v>
       </c>
       <c r="D111" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E111" t="s">
         <v>98</v>
@@ -4476,7 +4476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>

</xml_diff>